<commit_message>
Challenge 1 improved data tables.
</commit_message>
<xml_diff>
--- a/challenge1/challenge1.xlsx
+++ b/challenge1/challenge1.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/p3700621/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/p3700621/Coding/big-data-yelp-challenge/challenge1/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -1153,35 +1153,35 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$2:$A$221</c:f>
+              <c:f>Sheet1!$E$2:$E$286</c:f>
               <c:strCache>
-                <c:ptCount val="220"/>
+                <c:ptCount val="285"/>
                 <c:pt idx="0">
-                  <c:v>110. Las Vegas</c:v>
+                  <c:v>Ahwatukee</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Ahwatukee</c:v>
+                  <c:v>Allentown</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Ahwatukee Foothills Village</c:v>
+                  <c:v>Anjou</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Allegheny</c:v>
+                  <c:v>Anthem</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>Anjou</c:v>
+                  <c:v>Apache Junction</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>Anthem</c:v>
+                  <c:v>Arcadia</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>Apache Junction</c:v>
+                  <c:v>Aspinwall</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>Aspinwall</c:v>
+                  <c:v>Avondale</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>Avondale</c:v>
+                  <c:v>Baie-D'urfe</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>Beaconsfield</c:v>
@@ -1190,631 +1190,826 @@
                   <c:v>Bellevue</c:v>
                 </c:pt>
                 <c:pt idx="11">
+                  <c:v>Bellvue</c:v>
+                </c:pt>
+                <c:pt idx="12">
                   <c:v>Belmont</c:v>
                 </c:pt>
-                <c:pt idx="12">
-                  <c:v>Bethel Park</c:v>
-                </c:pt>
                 <c:pt idx="13">
+                  <c:v>Black Canyon City</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>Blainville</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>Blawnox</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>Bloomfield</c:v>
+                </c:pt>
+                <c:pt idx="17">
                   <c:v>Boisbriand</c:v>
                 </c:pt>
-                <c:pt idx="14">
-                  <c:v>Bonnyrigg</c:v>
-                </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="18">
+                  <c:v>Bonnyrigg and Lasswade</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>Boucherville</c:v>
+                </c:pt>
+                <c:pt idx="20">
                   <c:v>Boulder City</c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="21">
+                  <c:v>Braddock</c:v>
+                </c:pt>
+                <c:pt idx="22">
                   <c:v>Brentwood</c:v>
                 </c:pt>
-                <c:pt idx="17">
-                  <c:v>Breslau</c:v>
-                </c:pt>
-                <c:pt idx="18">
+                <c:pt idx="23">
                   <c:v>Bridgeville</c:v>
                 </c:pt>
-                <c:pt idx="19">
+                <c:pt idx="24">
+                  <c:v>Brookline</c:v>
+                </c:pt>
+                <c:pt idx="25">
                   <c:v>Brossard</c:v>
                 </c:pt>
-                <c:pt idx="20">
+                <c:pt idx="26">
                   <c:v>Buckeye</c:v>
                 </c:pt>
-                <c:pt idx="21">
-                  <c:v>Burbank</c:v>
-                </c:pt>
-                <c:pt idx="22">
+                <c:pt idx="27">
+                  <c:v>C Las Vegas</c:v>
+                </c:pt>
+                <c:pt idx="28">
                   <c:v>Cambridge</c:v>
                 </c:pt>
-                <c:pt idx="23">
+                <c:pt idx="29">
                   <c:v>Carefree</c:v>
                 </c:pt>
-                <c:pt idx="24">
+                <c:pt idx="30">
                   <c:v>Carnegie</c:v>
                 </c:pt>
-                <c:pt idx="25">
+                <c:pt idx="31">
                   <c:v>Casa Grande</c:v>
                 </c:pt>
-                <c:pt idx="26">
+                <c:pt idx="32">
                   <c:v>Castle Shannon</c:v>
                 </c:pt>
-                <c:pt idx="27">
+                <c:pt idx="33">
                   <c:v>Cave Creek</c:v>
                 </c:pt>
-                <c:pt idx="28">
-                  <c:v>Central City</c:v>
-                </c:pt>
-                <c:pt idx="29">
+                <c:pt idx="34">
+                  <c:v>Centennial Hills</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>Central</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>Central City Village</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>Central Henderson</c:v>
+                </c:pt>
+                <c:pt idx="38">
                   <c:v>Champaign</c:v>
                 </c:pt>
-                <c:pt idx="30">
+                <c:pt idx="39">
                   <c:v>Chandler</c:v>
                 </c:pt>
-                <c:pt idx="31">
+                <c:pt idx="40">
                   <c:v>Charlotte</c:v>
                 </c:pt>
-                <c:pt idx="32">
-                  <c:v>Charlotte</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>Chateau</c:v>
-                </c:pt>
-                <c:pt idx="34">
+                <c:pt idx="41">
                   <c:v>City of Edinburgh</c:v>
                 </c:pt>
-                <c:pt idx="35">
+                <c:pt idx="42">
                   <c:v>Clark</c:v>
                 </c:pt>
-                <c:pt idx="36">
-                  <c:v>Communauté-Urbaine-de-Montréal</c:v>
-                </c:pt>
-                <c:pt idx="37">
+                <c:pt idx="43">
+                  <c:v>Clover</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>Columbus</c:v>
+                </c:pt>
+                <c:pt idx="45">
                   <c:v>Concord</c:v>
                 </c:pt>
-                <c:pt idx="38">
+                <c:pt idx="46">
+                  <c:v>Concord Mills</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>Conestogo</c:v>
+                </c:pt>
+                <c:pt idx="48">
                   <c:v>Coolidge</c:v>
                 </c:pt>
-                <c:pt idx="39">
+                <c:pt idx="49">
+                  <c:v>Cornwell Development</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>Cote-Saint-Luc</c:v>
+                </c:pt>
+                <c:pt idx="51">
                   <c:v>Cottage Grove</c:v>
                 </c:pt>
-                <c:pt idx="40">
+                <c:pt idx="52">
                   <c:v>Crafton</c:v>
                 </c:pt>
-                <c:pt idx="41">
-                  <c:v>Cramond</c:v>
-                </c:pt>
-                <c:pt idx="42">
+                <c:pt idx="53">
+                  <c:v>Dalgety Bay</c:v>
+                </c:pt>
+                <c:pt idx="54">
                   <c:v>Dalkeith</c:v>
                 </c:pt>
-                <c:pt idx="43">
+                <c:pt idx="55">
+                  <c:v>Dallas</c:v>
+                </c:pt>
+                <c:pt idx="56">
                   <c:v>De Forest</c:v>
                 </c:pt>
-                <c:pt idx="44">
+                <c:pt idx="57">
                   <c:v>DeForest</c:v>
                 </c:pt>
-                <c:pt idx="45">
-                  <c:v>Deforest</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>Deux-Montagnes</c:v>
-                </c:pt>
-                <c:pt idx="47">
+                <c:pt idx="58">
+                  <c:v>Desert Ridge</c:v>
+                </c:pt>
+                <c:pt idx="59">
                   <c:v>Dollard-Des Ormeaux</c:v>
                 </c:pt>
-                <c:pt idx="48">
+                <c:pt idx="60">
                   <c:v>Dollard-Des-Ormeaux</c:v>
                 </c:pt>
-                <c:pt idx="49">
+                <c:pt idx="61">
                   <c:v>Dollard-des-Ormeaux</c:v>
                 </c:pt>
-                <c:pt idx="50">
+                <c:pt idx="62">
                   <c:v>Dormont</c:v>
                 </c:pt>
-                <c:pt idx="51">
+                <c:pt idx="63">
                   <c:v>Dorval</c:v>
                 </c:pt>
-                <c:pt idx="52">
+                <c:pt idx="64">
                   <c:v>Downtown</c:v>
                 </c:pt>
-                <c:pt idx="53">
+                <c:pt idx="65">
                   <c:v>Edgewood</c:v>
                 </c:pt>
-                <c:pt idx="54">
+                <c:pt idx="66">
                   <c:v>Edinburgh</c:v>
                 </c:pt>
-                <c:pt idx="55">
+                <c:pt idx="67">
+                  <c:v>Eggenstein-Leopoldshafen</c:v>
+                </c:pt>
+                <c:pt idx="68">
                   <c:v>El Mirage</c:v>
                 </c:pt>
-                <c:pt idx="56">
+                <c:pt idx="69">
                   <c:v>Enterprise</c:v>
                 </c:pt>
-                <c:pt idx="57">
-                  <c:v>Etna</c:v>
-                </c:pt>
-                <c:pt idx="58">
+                <c:pt idx="70">
                   <c:v>Ettlingen</c:v>
                 </c:pt>
-                <c:pt idx="59">
-                  <c:v>Fabreville</c:v>
-                </c:pt>
-                <c:pt idx="60">
+                <c:pt idx="71">
                   <c:v>Firth of Forth</c:v>
                 </c:pt>
-                <c:pt idx="61">
+                <c:pt idx="72">
                   <c:v>Fitchburg</c:v>
                 </c:pt>
-                <c:pt idx="62">
+                <c:pt idx="73">
                   <c:v>Florence</c:v>
                 </c:pt>
-                <c:pt idx="63">
+                <c:pt idx="74">
+                  <c:v>Fort Kinnaird</c:v>
+                </c:pt>
+                <c:pt idx="75">
                   <c:v>Fort McDowell</c:v>
                 </c:pt>
-                <c:pt idx="64">
+                <c:pt idx="76">
                   <c:v>Fort Mcdowell</c:v>
                 </c:pt>
-                <c:pt idx="65">
+                <c:pt idx="77">
                   <c:v>Fort Mill</c:v>
                 </c:pt>
-                <c:pt idx="66">
+                <c:pt idx="78">
+                  <c:v>Fort mill</c:v>
+                </c:pt>
+                <c:pt idx="79">
                   <c:v>Fountain Hills</c:v>
                 </c:pt>
-                <c:pt idx="67">
+                <c:pt idx="80">
+                  <c:v>Ft. Mill</c:v>
+                </c:pt>
+                <c:pt idx="81">
                   <c:v>Gila Bend</c:v>
                 </c:pt>
-                <c:pt idx="68">
+                <c:pt idx="82">
                   <c:v>Gilbert</c:v>
                 </c:pt>
-                <c:pt idx="69">
+                <c:pt idx="83">
                   <c:v>Glendale</c:v>
                 </c:pt>
-                <c:pt idx="70">
+                <c:pt idx="84">
+                  <c:v>Glendale Az</c:v>
+                </c:pt>
+                <c:pt idx="85">
                   <c:v>Gold Canyon</c:v>
                 </c:pt>
-                <c:pt idx="71">
-                  <c:v>Goldfield</c:v>
-                </c:pt>
-                <c:pt idx="72">
+                <c:pt idx="86">
+                  <c:v>Golden Square Mile</c:v>
+                </c:pt>
+                <c:pt idx="87">
                   <c:v>Goodyear</c:v>
                 </c:pt>
-                <c:pt idx="73">
-                  <c:v>Grand Canyon</c:v>
-                </c:pt>
-                <c:pt idx="74">
+                <c:pt idx="88">
+                  <c:v>Green Tree</c:v>
+                </c:pt>
+                <c:pt idx="89">
                   <c:v>Greenfield Park</c:v>
                 </c:pt>
-                <c:pt idx="75">
+                <c:pt idx="90">
                   <c:v>Guadalupe</c:v>
                 </c:pt>
-                <c:pt idx="76">
+                <c:pt idx="91">
                   <c:v>Harrisburg</c:v>
                 </c:pt>
-                <c:pt idx="77">
+                <c:pt idx="92">
+                  <c:v>Heidelberg</c:v>
+                </c:pt>
+                <c:pt idx="93">
                   <c:v>Henderson</c:v>
                 </c:pt>
-                <c:pt idx="78">
-                  <c:v>Henderson NV</c:v>
-                </c:pt>
-                <c:pt idx="79">
+                <c:pt idx="94">
+                  <c:v>Henderson and Las vegas</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>Henderston</c:v>
+                </c:pt>
+                <c:pt idx="96">
                   <c:v>Higley</c:v>
                 </c:pt>
-                <c:pt idx="80">
+                <c:pt idx="97">
                   <c:v>Homestead</c:v>
                 </c:pt>
-                <c:pt idx="81">
+                <c:pt idx="98">
                   <c:v>Huntersville</c:v>
                 </c:pt>
-                <c:pt idx="82">
-                  <c:v>Independence</c:v>
-                </c:pt>
-                <c:pt idx="83">
+                <c:pt idx="99">
                   <c:v>Indian Land</c:v>
                 </c:pt>
-                <c:pt idx="84">
+                <c:pt idx="100">
                   <c:v>Indian Trail</c:v>
                 </c:pt>
-                <c:pt idx="85">
-                  <c:v>Inverkeithing</c:v>
-                </c:pt>
-                <c:pt idx="86">
+                <c:pt idx="101">
                   <c:v>Juniper Green</c:v>
                 </c:pt>
-                <c:pt idx="87">
+                <c:pt idx="102">
                   <c:v>Karlsruhe</c:v>
                 </c:pt>
-                <c:pt idx="88">
+                <c:pt idx="103">
                   <c:v>Kirkland</c:v>
                 </c:pt>
-                <c:pt idx="89">
+                <c:pt idx="104">
                   <c:v>Kitchener</c:v>
                 </c:pt>
-                <c:pt idx="90">
-                  <c:v>L'Île-des-Soeurs</c:v>
-                </c:pt>
-                <c:pt idx="91">
+                <c:pt idx="105">
+                  <c:v>L'Île-Bizard</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>La Paz</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>La Prairie</c:v>
+                </c:pt>
+                <c:pt idx="108">
                   <c:v>LaSalle</c:v>
                 </c:pt>
-                <c:pt idx="92">
+                <c:pt idx="109">
                   <c:v>Lachine</c:v>
                 </c:pt>
-                <c:pt idx="93">
-                  <c:v>Lake Las Vegas</c:v>
-                </c:pt>
-                <c:pt idx="94">
+                <c:pt idx="110">
+                  <c:v>Lake Wylie</c:v>
+                </c:pt>
+                <c:pt idx="111">
                   <c:v>Las Vegas</c:v>
                 </c:pt>
-                <c:pt idx="95">
+                <c:pt idx="112">
                   <c:v>Las Vegas</c:v>
                 </c:pt>
-                <c:pt idx="96">
+                <c:pt idx="113">
+                  <c:v>Las Vegas, NV</c:v>
+                </c:pt>
+                <c:pt idx="114">
                   <c:v>Lasalle</c:v>
                 </c:pt>
-                <c:pt idx="97">
+                <c:pt idx="115">
                   <c:v>Lasswade</c:v>
                 </c:pt>
-                <c:pt idx="98">
+                <c:pt idx="116">
                   <c:v>Laval</c:v>
                 </c:pt>
-                <c:pt idx="99">
+                <c:pt idx="117">
                   <c:v>Laveen</c:v>
                 </c:pt>
-                <c:pt idx="100">
-                  <c:v>Laveen Village</c:v>
-                </c:pt>
-                <c:pt idx="101">
-                  <c:v>Le Sud-Ouest</c:v>
-                </c:pt>
-                <c:pt idx="102">
-                  <c:v>Le Vieux-Port</c:v>
-                </c:pt>
-                <c:pt idx="103">
+                <c:pt idx="118">
+                  <c:v>Lawrenceville</c:v>
+                </c:pt>
+                <c:pt idx="119">
                   <c:v>Leith</c:v>
                 </c:pt>
-                <c:pt idx="104">
+                <c:pt idx="120">
                   <c:v>Litchfield Park</c:v>
                 </c:pt>
-                <c:pt idx="105">
+                <c:pt idx="121">
+                  <c:v>Litchfield Park</c:v>
+                </c:pt>
+                <c:pt idx="122">
                   <c:v>Loanhead</c:v>
                 </c:pt>
-                <c:pt idx="106">
+                <c:pt idx="123">
                   <c:v>Longueuil</c:v>
                 </c:pt>
-                <c:pt idx="107">
-                  <c:v>MMRP</c:v>
-                </c:pt>
-                <c:pt idx="108">
+                <c:pt idx="124">
+                  <c:v>Lower Lawrenceville</c:v>
+                </c:pt>
+                <c:pt idx="125">
                   <c:v>Madison</c:v>
                 </c:pt>
-                <c:pt idx="109">
+                <c:pt idx="126">
                   <c:v>Maricopa</c:v>
                 </c:pt>
-                <c:pt idx="110">
-                  <c:v>Maricopa AZ</c:v>
-                </c:pt>
-                <c:pt idx="111">
+                <c:pt idx="127">
+                  <c:v>Mascouche</c:v>
+                </c:pt>
+                <c:pt idx="128">
+                  <c:v>Mattews</c:v>
+                </c:pt>
+                <c:pt idx="129">
                   <c:v>Matthews</c:v>
                 </c:pt>
-                <c:pt idx="112">
+                <c:pt idx="130">
                   <c:v>Mc Farland</c:v>
                 </c:pt>
-                <c:pt idx="113">
+                <c:pt idx="131">
                   <c:v>Mc Kees Rocks</c:v>
                 </c:pt>
-                <c:pt idx="114">
+                <c:pt idx="132">
+                  <c:v>McAdenville</c:v>
+                </c:pt>
+                <c:pt idx="133">
                   <c:v>McFarland</c:v>
                 </c:pt>
-                <c:pt idx="115">
+                <c:pt idx="134">
                   <c:v>McKees Rocks</c:v>
                 </c:pt>
-                <c:pt idx="116">
+                <c:pt idx="135">
+                  <c:v>McKeesport</c:v>
+                </c:pt>
+                <c:pt idx="136">
+                  <c:v>Mcfarland</c:v>
+                </c:pt>
+                <c:pt idx="137">
+                  <c:v>Mckees Rocks</c:v>
+                </c:pt>
+                <c:pt idx="138">
                   <c:v>Mesa</c:v>
                 </c:pt>
-                <c:pt idx="117">
-                  <c:v>Mesa</c:v>
-                </c:pt>
-                <c:pt idx="118">
-                  <c:v>Mesa AZ</c:v>
-                </c:pt>
-                <c:pt idx="119">
+                <c:pt idx="139">
                   <c:v>Middleton</c:v>
                 </c:pt>
-                <c:pt idx="120">
+                <c:pt idx="140">
+                  <c:v>Midlothian</c:v>
+                </c:pt>
+                <c:pt idx="141">
                   <c:v>Millvale</c:v>
                 </c:pt>
-                <c:pt idx="121">
+                <c:pt idx="142">
                   <c:v>Mint Hill</c:v>
                 </c:pt>
-                <c:pt idx="122">
+                <c:pt idx="143">
+                  <c:v>Mirabel</c:v>
+                </c:pt>
+                <c:pt idx="144">
                   <c:v>Monona</c:v>
                 </c:pt>
-                <c:pt idx="123">
+                <c:pt idx="145">
                   <c:v>Mont-Royal</c:v>
                 </c:pt>
-                <c:pt idx="124">
+                <c:pt idx="146">
                   <c:v>Montreal</c:v>
                 </c:pt>
-                <c:pt idx="125">
+                <c:pt idx="147">
+                  <c:v>Montreal-Est</c:v>
+                </c:pt>
+                <c:pt idx="148">
+                  <c:v>Montreal-Nord</c:v>
+                </c:pt>
+                <c:pt idx="149">
+                  <c:v>Montreal-Ouest</c:v>
+                </c:pt>
+                <c:pt idx="150">
+                  <c:v>Montreal-West</c:v>
+                </c:pt>
+                <c:pt idx="151">
                   <c:v>Montréal</c:v>
                 </c:pt>
-                <c:pt idx="126">
+                <c:pt idx="152">
+                  <c:v>Montréal-Nord</c:v>
+                </c:pt>
+                <c:pt idx="153">
+                  <c:v>Montréal-Ouest</c:v>
+                </c:pt>
+                <c:pt idx="154">
+                  <c:v>Montéal</c:v>
+                </c:pt>
+                <c:pt idx="155">
                   <c:v>Morristown</c:v>
                 </c:pt>
-                <c:pt idx="127">
+                <c:pt idx="156">
                   <c:v>Mount Holly</c:v>
                 </c:pt>
-                <c:pt idx="128">
+                <c:pt idx="157">
                   <c:v>Mount Lebanon</c:v>
                 </c:pt>
-                <c:pt idx="129">
+                <c:pt idx="158">
+                  <c:v>Mount Royal</c:v>
+                </c:pt>
+                <c:pt idx="159">
                   <c:v>Mount Washington</c:v>
                 </c:pt>
-                <c:pt idx="130">
+                <c:pt idx="160">
                   <c:v>Mt Lebanon</c:v>
                 </c:pt>
-                <c:pt idx="131">
+                <c:pt idx="161">
+                  <c:v>Mt. Oliver Boro</c:v>
+                </c:pt>
+                <c:pt idx="162">
                   <c:v>Munhall</c:v>
                 </c:pt>
-                <c:pt idx="132">
+                <c:pt idx="163">
                   <c:v>Musselburgh</c:v>
                 </c:pt>
-                <c:pt idx="133">
+                <c:pt idx="164">
+                  <c:v>N E Las Vegas</c:v>
+                </c:pt>
+                <c:pt idx="165">
                   <c:v>N Las Vegas</c:v>
                 </c:pt>
-                <c:pt idx="134">
+                <c:pt idx="166">
+                  <c:v>N W Las Vegas</c:v>
+                </c:pt>
+                <c:pt idx="167">
+                  <c:v>N. Las Vegas</c:v>
+                </c:pt>
+                <c:pt idx="168">
+                  <c:v>NELLIS AFB</c:v>
+                </c:pt>
+                <c:pt idx="169">
                   <c:v>Nellis AFB</c:v>
                 </c:pt>
-                <c:pt idx="135">
+                <c:pt idx="170">
                   <c:v>Nellis Afb</c:v>
                 </c:pt>
-                <c:pt idx="136">
-                  <c:v>Nellis Air Force Base</c:v>
-                </c:pt>
-                <c:pt idx="137">
-                  <c:v>New Town</c:v>
-                </c:pt>
-                <c:pt idx="138">
+                <c:pt idx="171">
+                  <c:v>New River</c:v>
+                </c:pt>
+                <c:pt idx="172">
                   <c:v>Newbridge</c:v>
                 </c:pt>
-                <c:pt idx="139">
+                <c:pt idx="173">
+                  <c:v>Newington</c:v>
+                </c:pt>
+                <c:pt idx="174">
                   <c:v>North Las Vegas</c:v>
                 </c:pt>
-                <c:pt idx="140">
+                <c:pt idx="175">
+                  <c:v>North Las Vegas</c:v>
+                </c:pt>
+                <c:pt idx="176">
+                  <c:v>North Queensferry</c:v>
+                </c:pt>
+                <c:pt idx="177">
+                  <c:v>North Scottsdale</c:v>
+                </c:pt>
+                <c:pt idx="178">
                   <c:v>Oakland</c:v>
                 </c:pt>
-                <c:pt idx="141">
-                  <c:v>Old Montreal</c:v>
-                </c:pt>
-                <c:pt idx="142">
+                <c:pt idx="179">
                   <c:v>Old Town</c:v>
                 </c:pt>
-                <c:pt idx="143">
+                <c:pt idx="180">
                   <c:v>Outremont</c:v>
                 </c:pt>
-                <c:pt idx="144">
+                <c:pt idx="181">
                   <c:v>Paradise</c:v>
                 </c:pt>
-                <c:pt idx="145">
+                <c:pt idx="182">
                   <c:v>Paradise Valley</c:v>
                 </c:pt>
-                <c:pt idx="146">
+                <c:pt idx="183">
+                  <c:v>Penicuik</c:v>
+                </c:pt>
+                <c:pt idx="184">
                   <c:v>Peoria</c:v>
                 </c:pt>
-                <c:pt idx="147">
+                <c:pt idx="185">
+                  <c:v>Pfinztal</c:v>
+                </c:pt>
+                <c:pt idx="186">
+                  <c:v>Pheonix</c:v>
+                </c:pt>
+                <c:pt idx="187">
                   <c:v>Phoenix</c:v>
                 </c:pt>
-                <c:pt idx="148">
-                  <c:v>Phoenix Sky Harbor Center</c:v>
-                </c:pt>
-                <c:pt idx="149">
+                <c:pt idx="188">
+                  <c:v>Phoenix-Ahwatukee</c:v>
+                </c:pt>
+                <c:pt idx="189">
                   <c:v>Pierrefonds</c:v>
                 </c:pt>
-                <c:pt idx="150">
+                <c:pt idx="190">
                   <c:v>Pineville</c:v>
                 </c:pt>
-                <c:pt idx="151">
+                <c:pt idx="191">
                   <c:v>Pittsburgh</c:v>
                 </c:pt>
-                <c:pt idx="152">
-                  <c:v>Pointe Claire</c:v>
-                </c:pt>
-                <c:pt idx="153">
+                <c:pt idx="192">
+                  <c:v>Pittsburgh/S. Hills Galleria</c:v>
+                </c:pt>
+                <c:pt idx="193">
+                  <c:v>Pittsburgh/Waterfront</c:v>
+                </c:pt>
+                <c:pt idx="194">
+                  <c:v>Pittsburrgh</c:v>
+                </c:pt>
+                <c:pt idx="195">
                   <c:v>Pointe-Aux-Trembles</c:v>
                 </c:pt>
-                <c:pt idx="154">
+                <c:pt idx="196">
                   <c:v>Pointe-Claire</c:v>
                 </c:pt>
-                <c:pt idx="155">
-                  <c:v>Portobello</c:v>
-                </c:pt>
-                <c:pt idx="156">
+                <c:pt idx="197">
                   <c:v>Queen Creek</c:v>
                 </c:pt>
-                <c:pt idx="157">
-                  <c:v>Rankin</c:v>
-                </c:pt>
-                <c:pt idx="158">
-                  <c:v>Regent Square</c:v>
-                </c:pt>
-                <c:pt idx="159">
+                <c:pt idx="198">
+                  <c:v>Queensferry</c:v>
+                </c:pt>
+                <c:pt idx="199">
+                  <c:v>Québec</c:v>
+                </c:pt>
+                <c:pt idx="200">
+                  <c:v>Ratho</c:v>
+                </c:pt>
+                <c:pt idx="201">
+                  <c:v>Rheinstetten</c:v>
+                </c:pt>
+                <c:pt idx="202">
                   <c:v>Rio Verde</c:v>
                 </c:pt>
-                <c:pt idx="160">
-                  <c:v>Roosevelt</c:v>
-                </c:pt>
-                <c:pt idx="161">
+                <c:pt idx="203">
+                  <c:v>Robinson Township</c:v>
+                </c:pt>
+                <c:pt idx="204">
+                  <c:v>Rock Hill</c:v>
+                </c:pt>
+                <c:pt idx="205">
+                  <c:v>Rockport</c:v>
+                </c:pt>
+                <c:pt idx="206">
                   <c:v>Rosemere</c:v>
                 </c:pt>
-                <c:pt idx="162">
+                <c:pt idx="207">
                   <c:v>Rosemère</c:v>
                 </c:pt>
-                <c:pt idx="163">
-                  <c:v>Roslin</c:v>
-                </c:pt>
-                <c:pt idx="164">
-                  <c:v>Saint Leonard</c:v>
-                </c:pt>
-                <c:pt idx="165">
+                <c:pt idx="208">
+                  <c:v>Roxboro</c:v>
+                </c:pt>
+                <c:pt idx="209">
+                  <c:v>Saint Laurent</c:v>
+                </c:pt>
+                <c:pt idx="210">
                   <c:v>Saint-Eustache</c:v>
                 </c:pt>
-                <c:pt idx="166">
-                  <c:v>Saint-Hubert</c:v>
-                </c:pt>
-                <c:pt idx="167">
+                <c:pt idx="211">
+                  <c:v>Saint-Henri</c:v>
+                </c:pt>
+                <c:pt idx="212">
                   <c:v>Saint-Lambert</c:v>
                 </c:pt>
-                <c:pt idx="168">
+                <c:pt idx="213">
                   <c:v>Saint-Laurent</c:v>
                 </c:pt>
-                <c:pt idx="169">
+                <c:pt idx="214">
                   <c:v>Saint-Leonard</c:v>
                 </c:pt>
-                <c:pt idx="170">
+                <c:pt idx="215">
+                  <c:v>Saint-laurent</c:v>
+                </c:pt>
+                <c:pt idx="216">
                   <c:v>Sainte-Anne-De-Bellevue</c:v>
                 </c:pt>
-                <c:pt idx="171">
+                <c:pt idx="217">
                   <c:v>Sainte-Anne-de-Bellevue</c:v>
                 </c:pt>
-                <c:pt idx="172">
-                  <c:v>Sainte-Therese</c:v>
-                </c:pt>
-                <c:pt idx="173">
+                <c:pt idx="218">
+                  <c:v>Sainte-Genevieve</c:v>
+                </c:pt>
+                <c:pt idx="219">
+                  <c:v>Sainte-Thérèse</c:v>
+                </c:pt>
+                <c:pt idx="220">
                   <c:v>San Tan Valley</c:v>
                 </c:pt>
-                <c:pt idx="174">
+                <c:pt idx="221">
                   <c:v>Savoy</c:v>
                 </c:pt>
-                <c:pt idx="175">
+                <c:pt idx="222">
+                  <c:v>Scottdale</c:v>
+                </c:pt>
+                <c:pt idx="223">
                   <c:v>Scottsdale</c:v>
                 </c:pt>
-                <c:pt idx="176">
-                  <c:v>South Gyle</c:v>
-                </c:pt>
-                <c:pt idx="177">
+                <c:pt idx="224">
+                  <c:v>Sedona</c:v>
+                </c:pt>
+                <c:pt idx="225">
+                  <c:v>Shady Side</c:v>
+                </c:pt>
+                <c:pt idx="226">
+                  <c:v>Shadyside</c:v>
+                </c:pt>
+                <c:pt idx="227">
+                  <c:v>Sharpsburg</c:v>
+                </c:pt>
+                <c:pt idx="228">
+                  <c:v>South Las Vegas</c:v>
+                </c:pt>
+                <c:pt idx="229">
+                  <c:v>South Mountain</c:v>
+                </c:pt>
+                <c:pt idx="230">
                   <c:v>South Queensferry</c:v>
                 </c:pt>
-                <c:pt idx="178">
-                  <c:v>Southside Flats</c:v>
-                </c:pt>
-                <c:pt idx="179">
+                <c:pt idx="231">
                   <c:v>Spring Valley</c:v>
                 </c:pt>
-                <c:pt idx="180">
-                  <c:v>St Leonard</c:v>
-                </c:pt>
-                <c:pt idx="181">
+                <c:pt idx="232">
+                  <c:v>Squirrel Hill</c:v>
+                </c:pt>
+                <c:pt idx="233">
+                  <c:v>St Jacobs</c:v>
+                </c:pt>
+                <c:pt idx="234">
                   <c:v>St. Jacobs</c:v>
                 </c:pt>
-                <c:pt idx="182">
-                  <c:v>Stanfield</c:v>
-                </c:pt>
-                <c:pt idx="183">
+                <c:pt idx="235">
+                  <c:v>Stallings</c:v>
+                </c:pt>
+                <c:pt idx="236">
+                  <c:v>Ste-Rose</c:v>
+                </c:pt>
+                <c:pt idx="237">
+                  <c:v>Stockbridge</c:v>
+                </c:pt>
+                <c:pt idx="238">
                   <c:v>Stoughton</c:v>
                 </c:pt>
-                <c:pt idx="184">
-                  <c:v>Summerlin South</c:v>
-                </c:pt>
-                <c:pt idx="185">
+                <c:pt idx="239">
+                  <c:v>Straiton</c:v>
+                </c:pt>
+                <c:pt idx="240">
+                  <c:v>Summerlin</c:v>
+                </c:pt>
+                <c:pt idx="241">
                   <c:v>Sun City</c:v>
                 </c:pt>
-                <c:pt idx="186">
-                  <c:v>Sun City Anthem</c:v>
-                </c:pt>
-                <c:pt idx="187">
+                <c:pt idx="242">
                   <c:v>Sun City West</c:v>
                 </c:pt>
-                <c:pt idx="188">
+                <c:pt idx="243">
                   <c:v>Sun Lakes</c:v>
                 </c:pt>
-                <c:pt idx="189">
+                <c:pt idx="244">
                   <c:v>Sun Prairie</c:v>
                 </c:pt>
-                <c:pt idx="190">
+                <c:pt idx="245">
+                  <c:v>Sunrise</c:v>
+                </c:pt>
+                <c:pt idx="246">
                   <c:v>Surprise</c:v>
                 </c:pt>
-                <c:pt idx="191">
-                  <c:v>Surprise Crossing</c:v>
-                </c:pt>
-                <c:pt idx="192">
+                <c:pt idx="247">
+                  <c:v>Swissvale</c:v>
+                </c:pt>
+                <c:pt idx="248">
                   <c:v>Tega Cay</c:v>
                 </c:pt>
-                <c:pt idx="193">
+                <c:pt idx="249">
                   <c:v>Tempe</c:v>
                 </c:pt>
-                <c:pt idx="194">
+                <c:pt idx="250">
+                  <c:v>Terrebonne</c:v>
+                </c:pt>
+                <c:pt idx="251">
                   <c:v>Tolleson</c:v>
                 </c:pt>
-                <c:pt idx="195">
+                <c:pt idx="252">
                   <c:v>Tonopah</c:v>
                 </c:pt>
-                <c:pt idx="196">
+                <c:pt idx="253">
                   <c:v>Tonto Basin</c:v>
                 </c:pt>
-                <c:pt idx="197">
+                <c:pt idx="254">
                   <c:v>Tortilla Flat</c:v>
                 </c:pt>
-                <c:pt idx="198">
+                <c:pt idx="255">
+                  <c:v>University</c:v>
+                </c:pt>
+                <c:pt idx="256">
+                  <c:v>Upper Saint Clair</c:v>
+                </c:pt>
+                <c:pt idx="257">
                   <c:v>Urbana</c:v>
                 </c:pt>
-                <c:pt idx="199">
+                <c:pt idx="258">
                   <c:v>Verdun</c:v>
                 </c:pt>
-                <c:pt idx="200">
+                <c:pt idx="259">
                   <c:v>Verona</c:v>
                 </c:pt>
-                <c:pt idx="201">
+                <c:pt idx="260">
+                  <c:v>Victoria Park</c:v>
+                </c:pt>
+                <c:pt idx="261">
                   <c:v>Vimont</c:v>
                 </c:pt>
-                <c:pt idx="202">
+                <c:pt idx="262">
+                  <c:v>W Henderson</c:v>
+                </c:pt>
+                <c:pt idx="263">
+                  <c:v>W Spring Valley</c:v>
+                </c:pt>
+                <c:pt idx="264">
+                  <c:v>W Summerlin</c:v>
+                </c:pt>
+                <c:pt idx="265">
                   <c:v>Waddell</c:v>
                 </c:pt>
-                <c:pt idx="203">
-                  <c:v>Water of Leith</c:v>
-                </c:pt>
-                <c:pt idx="204">
+                <c:pt idx="266">
+                  <c:v>Waldbronn</c:v>
+                </c:pt>
+                <c:pt idx="267">
                   <c:v>Waterloo</c:v>
                 </c:pt>
-                <c:pt idx="205">
+                <c:pt idx="268">
                   <c:v>Waunakee</c:v>
                 </c:pt>
-                <c:pt idx="206">
+                <c:pt idx="269">
                   <c:v>Waxhaw</c:v>
                 </c:pt>
-                <c:pt idx="207">
+                <c:pt idx="270">
                   <c:v>Weddington</c:v>
                 </c:pt>
-                <c:pt idx="208">
+                <c:pt idx="271">
+                  <c:v>Weingarten</c:v>
+                </c:pt>
+                <c:pt idx="272">
                   <c:v>Wesley Chapel</c:v>
                 </c:pt>
-                <c:pt idx="209">
+                <c:pt idx="273">
                   <c:v>West Homestead</c:v>
                 </c:pt>
-                <c:pt idx="210">
+                <c:pt idx="274">
                   <c:v>West Mifflin</c:v>
                 </c:pt>
-                <c:pt idx="211">
+                <c:pt idx="275">
                   <c:v>Westmount</c:v>
                 </c:pt>
-                <c:pt idx="212">
-                  <c:v>Westworld Scottsdale</c:v>
-                </c:pt>
-                <c:pt idx="213">
-                  <c:v>Whitney</c:v>
-                </c:pt>
-                <c:pt idx="214">
+                <c:pt idx="276">
+                  <c:v>Whitehall</c:v>
+                </c:pt>
+                <c:pt idx="277">
                   <c:v>Wickenburg</c:v>
                 </c:pt>
-                <c:pt idx="215">
+                <c:pt idx="278">
                   <c:v>Wilkinsburg</c:v>
                 </c:pt>
-                <c:pt idx="216">
+                <c:pt idx="279">
                   <c:v>Windsor</c:v>
                 </c:pt>
-                <c:pt idx="217">
-                  <c:v>Wittmann</c:v>
-                </c:pt>
-                <c:pt idx="218">
+                <c:pt idx="280">
+                  <c:v>Wörth am Rhein</c:v>
+                </c:pt>
+                <c:pt idx="281">
                   <c:v>Youngtown</c:v>
                 </c:pt>
-                <c:pt idx="219">
-                  <c:v>chandler</c:v>
+                <c:pt idx="282">
+                  <c:v>glendale</c:v>
+                </c:pt>
+                <c:pt idx="283">
+                  <c:v>rankin</c:v>
+                </c:pt>
+                <c:pt idx="284">
+                  <c:v>Île des Soeurs</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2516,6 +2711,869 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$E$2:$E$286</c:f>
+              <c:strCache>
+                <c:ptCount val="285"/>
+                <c:pt idx="0">
+                  <c:v>Ahwatukee</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Allentown</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Anjou</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Anthem</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Apache Junction</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Arcadia</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Aspinwall</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Avondale</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Baie-D'urfe</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Beaconsfield</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Bellevue</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Bellvue</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>Belmont</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>Black Canyon City</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>Blainville</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>Blawnox</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>Bloomfield</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>Boisbriand</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>Bonnyrigg and Lasswade</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>Boucherville</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>Boulder City</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>Braddock</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>Brentwood</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>Bridgeville</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>Brookline</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>Brossard</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>Buckeye</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>C Las Vegas</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>Cambridge</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>Carefree</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>Carnegie</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>Casa Grande</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>Castle Shannon</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>Cave Creek</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>Centennial Hills</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>Central</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>Central City Village</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>Central Henderson</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>Champaign</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>Chandler</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>Charlotte</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>City of Edinburgh</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>Clark</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>Clover</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>Columbus</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>Concord</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>Concord Mills</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>Conestogo</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>Coolidge</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>Cornwell Development</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>Cote-Saint-Luc</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>Cottage Grove</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>Crafton</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>Dalgety Bay</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>Dalkeith</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>Dallas</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>De Forest</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>DeForest</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>Desert Ridge</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>Dollard-Des Ormeaux</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>Dollard-Des-Ormeaux</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>Dollard-des-Ormeaux</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>Dormont</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>Dorval</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>Downtown</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>Edgewood</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>Edinburgh</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>Eggenstein-Leopoldshafen</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>El Mirage</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>Enterprise</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>Ettlingen</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>Firth of Forth</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>Fitchburg</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>Florence</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>Fort Kinnaird</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>Fort McDowell</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>Fort Mcdowell</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>Fort Mill</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>Fort mill</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>Fountain Hills</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>Ft. Mill</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>Gila Bend</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>Gilbert</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>Glendale</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>Glendale Az</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>Gold Canyon</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>Golden Square Mile</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>Goodyear</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>Green Tree</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>Greenfield Park</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>Guadalupe</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>Harrisburg</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>Heidelberg</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>Henderson</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>Henderson and Las vegas</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>Henderston</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>Higley</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>Homestead</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>Huntersville</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>Indian Land</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>Indian Trail</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>Juniper Green</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>Karlsruhe</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>Kirkland</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>Kitchener</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>L'Île-Bizard</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>La Paz</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>La Prairie</c:v>
+                </c:pt>
+                <c:pt idx="108">
+                  <c:v>LaSalle</c:v>
+                </c:pt>
+                <c:pt idx="109">
+                  <c:v>Lachine</c:v>
+                </c:pt>
+                <c:pt idx="110">
+                  <c:v>Lake Wylie</c:v>
+                </c:pt>
+                <c:pt idx="111">
+                  <c:v>Las Vegas</c:v>
+                </c:pt>
+                <c:pt idx="112">
+                  <c:v>Las Vegas</c:v>
+                </c:pt>
+                <c:pt idx="113">
+                  <c:v>Las Vegas, NV</c:v>
+                </c:pt>
+                <c:pt idx="114">
+                  <c:v>Lasalle</c:v>
+                </c:pt>
+                <c:pt idx="115">
+                  <c:v>Lasswade</c:v>
+                </c:pt>
+                <c:pt idx="116">
+                  <c:v>Laval</c:v>
+                </c:pt>
+                <c:pt idx="117">
+                  <c:v>Laveen</c:v>
+                </c:pt>
+                <c:pt idx="118">
+                  <c:v>Lawrenceville</c:v>
+                </c:pt>
+                <c:pt idx="119">
+                  <c:v>Leith</c:v>
+                </c:pt>
+                <c:pt idx="120">
+                  <c:v>Litchfield Park</c:v>
+                </c:pt>
+                <c:pt idx="121">
+                  <c:v>Litchfield Park</c:v>
+                </c:pt>
+                <c:pt idx="122">
+                  <c:v>Loanhead</c:v>
+                </c:pt>
+                <c:pt idx="123">
+                  <c:v>Longueuil</c:v>
+                </c:pt>
+                <c:pt idx="124">
+                  <c:v>Lower Lawrenceville</c:v>
+                </c:pt>
+                <c:pt idx="125">
+                  <c:v>Madison</c:v>
+                </c:pt>
+                <c:pt idx="126">
+                  <c:v>Maricopa</c:v>
+                </c:pt>
+                <c:pt idx="127">
+                  <c:v>Mascouche</c:v>
+                </c:pt>
+                <c:pt idx="128">
+                  <c:v>Mattews</c:v>
+                </c:pt>
+                <c:pt idx="129">
+                  <c:v>Matthews</c:v>
+                </c:pt>
+                <c:pt idx="130">
+                  <c:v>Mc Farland</c:v>
+                </c:pt>
+                <c:pt idx="131">
+                  <c:v>Mc Kees Rocks</c:v>
+                </c:pt>
+                <c:pt idx="132">
+                  <c:v>McAdenville</c:v>
+                </c:pt>
+                <c:pt idx="133">
+                  <c:v>McFarland</c:v>
+                </c:pt>
+                <c:pt idx="134">
+                  <c:v>McKees Rocks</c:v>
+                </c:pt>
+                <c:pt idx="135">
+                  <c:v>McKeesport</c:v>
+                </c:pt>
+                <c:pt idx="136">
+                  <c:v>Mcfarland</c:v>
+                </c:pt>
+                <c:pt idx="137">
+                  <c:v>Mckees Rocks</c:v>
+                </c:pt>
+                <c:pt idx="138">
+                  <c:v>Mesa</c:v>
+                </c:pt>
+                <c:pt idx="139">
+                  <c:v>Middleton</c:v>
+                </c:pt>
+                <c:pt idx="140">
+                  <c:v>Midlothian</c:v>
+                </c:pt>
+                <c:pt idx="141">
+                  <c:v>Millvale</c:v>
+                </c:pt>
+                <c:pt idx="142">
+                  <c:v>Mint Hill</c:v>
+                </c:pt>
+                <c:pt idx="143">
+                  <c:v>Mirabel</c:v>
+                </c:pt>
+                <c:pt idx="144">
+                  <c:v>Monona</c:v>
+                </c:pt>
+                <c:pt idx="145">
+                  <c:v>Mont-Royal</c:v>
+                </c:pt>
+                <c:pt idx="146">
+                  <c:v>Montreal</c:v>
+                </c:pt>
+                <c:pt idx="147">
+                  <c:v>Montreal-Est</c:v>
+                </c:pt>
+                <c:pt idx="148">
+                  <c:v>Montreal-Nord</c:v>
+                </c:pt>
+                <c:pt idx="149">
+                  <c:v>Montreal-Ouest</c:v>
+                </c:pt>
+                <c:pt idx="150">
+                  <c:v>Montreal-West</c:v>
+                </c:pt>
+                <c:pt idx="151">
+                  <c:v>Montréal</c:v>
+                </c:pt>
+                <c:pt idx="152">
+                  <c:v>Montréal-Nord</c:v>
+                </c:pt>
+                <c:pt idx="153">
+                  <c:v>Montréal-Ouest</c:v>
+                </c:pt>
+                <c:pt idx="154">
+                  <c:v>Montéal</c:v>
+                </c:pt>
+                <c:pt idx="155">
+                  <c:v>Morristown</c:v>
+                </c:pt>
+                <c:pt idx="156">
+                  <c:v>Mount Holly</c:v>
+                </c:pt>
+                <c:pt idx="157">
+                  <c:v>Mount Lebanon</c:v>
+                </c:pt>
+                <c:pt idx="158">
+                  <c:v>Mount Royal</c:v>
+                </c:pt>
+                <c:pt idx="159">
+                  <c:v>Mount Washington</c:v>
+                </c:pt>
+                <c:pt idx="160">
+                  <c:v>Mt Lebanon</c:v>
+                </c:pt>
+                <c:pt idx="161">
+                  <c:v>Mt. Oliver Boro</c:v>
+                </c:pt>
+                <c:pt idx="162">
+                  <c:v>Munhall</c:v>
+                </c:pt>
+                <c:pt idx="163">
+                  <c:v>Musselburgh</c:v>
+                </c:pt>
+                <c:pt idx="164">
+                  <c:v>N E Las Vegas</c:v>
+                </c:pt>
+                <c:pt idx="165">
+                  <c:v>N Las Vegas</c:v>
+                </c:pt>
+                <c:pt idx="166">
+                  <c:v>N W Las Vegas</c:v>
+                </c:pt>
+                <c:pt idx="167">
+                  <c:v>N. Las Vegas</c:v>
+                </c:pt>
+                <c:pt idx="168">
+                  <c:v>NELLIS AFB</c:v>
+                </c:pt>
+                <c:pt idx="169">
+                  <c:v>Nellis AFB</c:v>
+                </c:pt>
+                <c:pt idx="170">
+                  <c:v>Nellis Afb</c:v>
+                </c:pt>
+                <c:pt idx="171">
+                  <c:v>New River</c:v>
+                </c:pt>
+                <c:pt idx="172">
+                  <c:v>Newbridge</c:v>
+                </c:pt>
+                <c:pt idx="173">
+                  <c:v>Newington</c:v>
+                </c:pt>
+                <c:pt idx="174">
+                  <c:v>North Las Vegas</c:v>
+                </c:pt>
+                <c:pt idx="175">
+                  <c:v>North Las Vegas</c:v>
+                </c:pt>
+                <c:pt idx="176">
+                  <c:v>North Queensferry</c:v>
+                </c:pt>
+                <c:pt idx="177">
+                  <c:v>North Scottsdale</c:v>
+                </c:pt>
+                <c:pt idx="178">
+                  <c:v>Oakland</c:v>
+                </c:pt>
+                <c:pt idx="179">
+                  <c:v>Old Town</c:v>
+                </c:pt>
+                <c:pt idx="180">
+                  <c:v>Outremont</c:v>
+                </c:pt>
+                <c:pt idx="181">
+                  <c:v>Paradise</c:v>
+                </c:pt>
+                <c:pt idx="182">
+                  <c:v>Paradise Valley</c:v>
+                </c:pt>
+                <c:pt idx="183">
+                  <c:v>Penicuik</c:v>
+                </c:pt>
+                <c:pt idx="184">
+                  <c:v>Peoria</c:v>
+                </c:pt>
+                <c:pt idx="185">
+                  <c:v>Pfinztal</c:v>
+                </c:pt>
+                <c:pt idx="186">
+                  <c:v>Pheonix</c:v>
+                </c:pt>
+                <c:pt idx="187">
+                  <c:v>Phoenix</c:v>
+                </c:pt>
+                <c:pt idx="188">
+                  <c:v>Phoenix-Ahwatukee</c:v>
+                </c:pt>
+                <c:pt idx="189">
+                  <c:v>Pierrefonds</c:v>
+                </c:pt>
+                <c:pt idx="190">
+                  <c:v>Pineville</c:v>
+                </c:pt>
+                <c:pt idx="191">
+                  <c:v>Pittsburgh</c:v>
+                </c:pt>
+                <c:pt idx="192">
+                  <c:v>Pittsburgh/S. Hills Galleria</c:v>
+                </c:pt>
+                <c:pt idx="193">
+                  <c:v>Pittsburgh/Waterfront</c:v>
+                </c:pt>
+                <c:pt idx="194">
+                  <c:v>Pittsburrgh</c:v>
+                </c:pt>
+                <c:pt idx="195">
+                  <c:v>Pointe-Aux-Trembles</c:v>
+                </c:pt>
+                <c:pt idx="196">
+                  <c:v>Pointe-Claire</c:v>
+                </c:pt>
+                <c:pt idx="197">
+                  <c:v>Queen Creek</c:v>
+                </c:pt>
+                <c:pt idx="198">
+                  <c:v>Queensferry</c:v>
+                </c:pt>
+                <c:pt idx="199">
+                  <c:v>Québec</c:v>
+                </c:pt>
+                <c:pt idx="200">
+                  <c:v>Ratho</c:v>
+                </c:pt>
+                <c:pt idx="201">
+                  <c:v>Rheinstetten</c:v>
+                </c:pt>
+                <c:pt idx="202">
+                  <c:v>Rio Verde</c:v>
+                </c:pt>
+                <c:pt idx="203">
+                  <c:v>Robinson Township</c:v>
+                </c:pt>
+                <c:pt idx="204">
+                  <c:v>Rock Hill</c:v>
+                </c:pt>
+                <c:pt idx="205">
+                  <c:v>Rockport</c:v>
+                </c:pt>
+                <c:pt idx="206">
+                  <c:v>Rosemere</c:v>
+                </c:pt>
+                <c:pt idx="207">
+                  <c:v>Rosemère</c:v>
+                </c:pt>
+                <c:pt idx="208">
+                  <c:v>Roxboro</c:v>
+                </c:pt>
+                <c:pt idx="209">
+                  <c:v>Saint Laurent</c:v>
+                </c:pt>
+                <c:pt idx="210">
+                  <c:v>Saint-Eustache</c:v>
+                </c:pt>
+                <c:pt idx="211">
+                  <c:v>Saint-Henri</c:v>
+                </c:pt>
+                <c:pt idx="212">
+                  <c:v>Saint-Lambert</c:v>
+                </c:pt>
+                <c:pt idx="213">
+                  <c:v>Saint-Laurent</c:v>
+                </c:pt>
+                <c:pt idx="214">
+                  <c:v>Saint-Leonard</c:v>
+                </c:pt>
+                <c:pt idx="215">
+                  <c:v>Saint-laurent</c:v>
+                </c:pt>
+                <c:pt idx="216">
+                  <c:v>Sainte-Anne-De-Bellevue</c:v>
+                </c:pt>
+                <c:pt idx="217">
+                  <c:v>Sainte-Anne-de-Bellevue</c:v>
+                </c:pt>
+                <c:pt idx="218">
+                  <c:v>Sainte-Genevieve</c:v>
+                </c:pt>
+                <c:pt idx="219">
+                  <c:v>Sainte-Thérèse</c:v>
+                </c:pt>
+                <c:pt idx="220">
+                  <c:v>San Tan Valley</c:v>
+                </c:pt>
+                <c:pt idx="221">
+                  <c:v>Savoy</c:v>
+                </c:pt>
+                <c:pt idx="222">
+                  <c:v>Scottdale</c:v>
+                </c:pt>
+                <c:pt idx="223">
+                  <c:v>Scottsdale</c:v>
+                </c:pt>
+                <c:pt idx="224">
+                  <c:v>Sedona</c:v>
+                </c:pt>
+                <c:pt idx="225">
+                  <c:v>Shady Side</c:v>
+                </c:pt>
+                <c:pt idx="226">
+                  <c:v>Shadyside</c:v>
+                </c:pt>
+                <c:pt idx="227">
+                  <c:v>Sharpsburg</c:v>
+                </c:pt>
+                <c:pt idx="228">
+                  <c:v>South Las Vegas</c:v>
+                </c:pt>
+                <c:pt idx="229">
+                  <c:v>South Mountain</c:v>
+                </c:pt>
+                <c:pt idx="230">
+                  <c:v>South Queensferry</c:v>
+                </c:pt>
+                <c:pt idx="231">
+                  <c:v>Spring Valley</c:v>
+                </c:pt>
+                <c:pt idx="232">
+                  <c:v>Squirrel Hill</c:v>
+                </c:pt>
+                <c:pt idx="233">
+                  <c:v>St Jacobs</c:v>
+                </c:pt>
+                <c:pt idx="234">
+                  <c:v>St. Jacobs</c:v>
+                </c:pt>
+                <c:pt idx="235">
+                  <c:v>Stallings</c:v>
+                </c:pt>
+                <c:pt idx="236">
+                  <c:v>Ste-Rose</c:v>
+                </c:pt>
+                <c:pt idx="237">
+                  <c:v>Stockbridge</c:v>
+                </c:pt>
+                <c:pt idx="238">
+                  <c:v>Stoughton</c:v>
+                </c:pt>
+                <c:pt idx="239">
+                  <c:v>Straiton</c:v>
+                </c:pt>
+                <c:pt idx="240">
+                  <c:v>Summerlin</c:v>
+                </c:pt>
+                <c:pt idx="241">
+                  <c:v>Sun City</c:v>
+                </c:pt>
+                <c:pt idx="242">
+                  <c:v>Sun City West</c:v>
+                </c:pt>
+                <c:pt idx="243">
+                  <c:v>Sun Lakes</c:v>
+                </c:pt>
+                <c:pt idx="244">
+                  <c:v>Sun Prairie</c:v>
+                </c:pt>
+                <c:pt idx="245">
+                  <c:v>Sunrise</c:v>
+                </c:pt>
+                <c:pt idx="246">
+                  <c:v>Surprise</c:v>
+                </c:pt>
+                <c:pt idx="247">
+                  <c:v>Swissvale</c:v>
+                </c:pt>
+                <c:pt idx="248">
+                  <c:v>Tega Cay</c:v>
+                </c:pt>
+                <c:pt idx="249">
+                  <c:v>Tempe</c:v>
+                </c:pt>
+                <c:pt idx="250">
+                  <c:v>Terrebonne</c:v>
+                </c:pt>
+                <c:pt idx="251">
+                  <c:v>Tolleson</c:v>
+                </c:pt>
+                <c:pt idx="252">
+                  <c:v>Tonopah</c:v>
+                </c:pt>
+                <c:pt idx="253">
+                  <c:v>Tonto Basin</c:v>
+                </c:pt>
+                <c:pt idx="254">
+                  <c:v>Tortilla Flat</c:v>
+                </c:pt>
+                <c:pt idx="255">
+                  <c:v>University</c:v>
+                </c:pt>
+                <c:pt idx="256">
+                  <c:v>Upper Saint Clair</c:v>
+                </c:pt>
+                <c:pt idx="257">
+                  <c:v>Urbana</c:v>
+                </c:pt>
+                <c:pt idx="258">
+                  <c:v>Verdun</c:v>
+                </c:pt>
+                <c:pt idx="259">
+                  <c:v>Verona</c:v>
+                </c:pt>
+                <c:pt idx="260">
+                  <c:v>Victoria Park</c:v>
+                </c:pt>
+                <c:pt idx="261">
+                  <c:v>Vimont</c:v>
+                </c:pt>
+                <c:pt idx="262">
+                  <c:v>W Henderson</c:v>
+                </c:pt>
+                <c:pt idx="263">
+                  <c:v>W Spring Valley</c:v>
+                </c:pt>
+                <c:pt idx="264">
+                  <c:v>W Summerlin</c:v>
+                </c:pt>
+                <c:pt idx="265">
+                  <c:v>Waddell</c:v>
+                </c:pt>
+                <c:pt idx="266">
+                  <c:v>Waldbronn</c:v>
+                </c:pt>
+                <c:pt idx="267">
+                  <c:v>Waterloo</c:v>
+                </c:pt>
+                <c:pt idx="268">
+                  <c:v>Waunakee</c:v>
+                </c:pt>
+                <c:pt idx="269">
+                  <c:v>Waxhaw</c:v>
+                </c:pt>
+                <c:pt idx="270">
+                  <c:v>Weddington</c:v>
+                </c:pt>
+                <c:pt idx="271">
+                  <c:v>Weingarten</c:v>
+                </c:pt>
+                <c:pt idx="272">
+                  <c:v>Wesley Chapel</c:v>
+                </c:pt>
+                <c:pt idx="273">
+                  <c:v>West Homestead</c:v>
+                </c:pt>
+                <c:pt idx="274">
+                  <c:v>West Mifflin</c:v>
+                </c:pt>
+                <c:pt idx="275">
+                  <c:v>Westmount</c:v>
+                </c:pt>
+                <c:pt idx="276">
+                  <c:v>Whitehall</c:v>
+                </c:pt>
+                <c:pt idx="277">
+                  <c:v>Wickenburg</c:v>
+                </c:pt>
+                <c:pt idx="278">
+                  <c:v>Wilkinsburg</c:v>
+                </c:pt>
+                <c:pt idx="279">
+                  <c:v>Windsor</c:v>
+                </c:pt>
+                <c:pt idx="280">
+                  <c:v>Wörth am Rhein</c:v>
+                </c:pt>
+                <c:pt idx="281">
+                  <c:v>Youngtown</c:v>
+                </c:pt>
+                <c:pt idx="282">
+                  <c:v>glendale</c:v>
+                </c:pt>
+                <c:pt idx="283">
+                  <c:v>rankin</c:v>
+                </c:pt>
+                <c:pt idx="284">
+                  <c:v>Île des Soeurs</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
           <c:val>
             <c:numRef>
               <c:f>Sheet1!$F$2:$F$221</c:f>
@@ -3196,11 +4254,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-2104600976"/>
-        <c:axId val="-2104599568"/>
+        <c:axId val="-2144055568"/>
+        <c:axId val="-2145358432"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2104600976"/>
+        <c:axId val="-2144055568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3243,7 +4301,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2104599568"/>
+        <c:crossAx val="-2145358432"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3251,7 +4309,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2104599568"/>
+        <c:axId val="-2145358432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3301,7 +4359,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2104600976"/>
+        <c:crossAx val="-2144055568"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4206,8 +5264,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A96" sqref="A96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>

</xml_diff>